<commit_message>
tabelle angepasst, aufgaben als todos in quellcode
</commit_message>
<xml_diff>
--- a/Teilaufgaben.xlsx
+++ b/Teilaufgaben.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Hilfefunktion (PDF per Button öffnen)</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Interruptfunktion (mind. TMR- und RB0-Interrupt)</t>
+  </si>
+  <si>
+    <t>Testprogramm 1</t>
+  </si>
+  <si>
+    <t>Testprogramm 2</t>
+  </si>
+  <si>
+    <t>Erreichte Punkte</t>
   </si>
 </sst>
 </file>
@@ -149,10 +158,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -447,193 +457,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.140625" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C2" s="3"/>
+      <c r="D2" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3">
         <v>10</v>
       </c>
-      <c r="D1" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1">
+      <c r="A4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1">
+      <c r="C6" s="3"/>
+      <c r="D6" s="1">
         <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="1" customFormat="1">
-      <c r="A18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="1">
-        <v>40</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="1" customFormat="1">
+      <c r="A21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="1">
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B22">
         <v>5</v>
@@ -641,88 +661,112 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B25">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B26">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="1" customFormat="1">
-      <c r="A28" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="1">
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
+    <row r="31" spans="1:4" s="1" customFormat="1">
+      <c r="A31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
         <v>27</v>
       </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" s="1" customFormat="1">
-      <c r="A34" s="1" t="s">
+      <c r="B35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" s="1" customFormat="1">
+      <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C34">
-        <f>SUM(C1:C32)</f>
-        <v>22</v>
-      </c>
-      <c r="D34" s="1">
+      <c r="C37">
+        <f>SUM(C2:C35)</f>
+        <v>32</v>
+      </c>
+      <c r="D37" s="1">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pc funktionen implementiert (testfile7), timerinterrupt begonnen, comport-java file noch ohne funktion
</commit_message>
<xml_diff>
--- a/Teilaufgaben.xlsx
+++ b/Teilaufgaben.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="18990" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Hilfefunktion (PDF per Button öffnen)</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Erreichte Punkte</t>
+  </si>
+  <si>
+    <t>Was läuft durch?</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -457,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -468,14 +474,15 @@
     <col min="1" max="1" width="54.140625" customWidth="1"/>
     <col min="2" max="2" width="3.85546875" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="C1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1">
+    <row r="2" spans="1:7" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -483,8 +490,11 @@
       <c r="D2" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1">
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
@@ -495,8 +505,14 @@
         <v>10</v>
       </c>
       <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1">
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -507,12 +523,22 @@
         <v>10</v>
       </c>
       <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" s="3">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1">
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -520,8 +546,12 @@
       <c r="D6" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -531,8 +561,12 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="F7" s="3">
+        <v>6</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -542,16 +576,26 @@
       <c r="C8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="F8" s="3">
+        <v>7</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="F9" s="3">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -561,24 +605,34 @@
       <c r="C10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="F10" s="3">
+        <v>9</v>
+      </c>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -586,7 +640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -594,7 +648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -602,7 +656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -764,7 +818,7 @@
       </c>
       <c r="C37">
         <f>SUM(C2:C35)</f>
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D37" s="1">
         <v>100</v>

</xml_diff>

<commit_message>
gui überarbeitet, thread  geändert (läuft stabiler), neue befehle implementiert, interrupts implementiert ...
</commit_message>
<xml_diff>
--- a/Teilaufgaben.xlsx
+++ b/Teilaufgaben.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Hilfefunktion (PDF per Button öffnen)</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>------------</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -164,11 +170,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -465,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -536,7 +543,9 @@
       <c r="F5" s="3">
         <v>3</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
@@ -590,6 +599,9 @@
       <c r="B9">
         <v>1</v>
       </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
       <c r="F9" s="3">
         <v>8</v>
       </c>
@@ -639,6 +651,9 @@
       <c r="B13">
         <v>4</v>
       </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
@@ -647,6 +662,9 @@
       <c r="B14">
         <v>2</v>
       </c>
+      <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
@@ -655,6 +673,9 @@
       <c r="B15">
         <v>1</v>
       </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
@@ -663,6 +684,9 @@
       <c r="B16">
         <v>5</v>
       </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
@@ -744,6 +768,9 @@
       <c r="B26">
         <v>5</v>
       </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
@@ -818,7 +845,7 @@
       </c>
       <c r="C37">
         <f>SUM(C2:C35)</f>
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D37" s="1">
         <v>100</v>

</xml_diff>

<commit_message>
externer Clock zum Teil implementiert
</commit_message>
<xml_diff>
--- a/Teilaufgaben.xlsx
+++ b/Teilaufgaben.xlsx
@@ -150,12 +150,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -170,12 +176,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -472,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -508,7 +516,7 @@
       <c r="B3" s="3">
         <v>10</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>10</v>
       </c>
       <c r="D3" s="2"/>
@@ -526,7 +534,7 @@
       <c r="B4" s="3">
         <v>10</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>10</v>
       </c>
       <c r="D4" s="2"/>
@@ -540,6 +548,10 @@
     <row r="5" spans="1:7">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
+      <c r="D5">
+        <f>SUM(C3:C4)</f>
+        <v>20</v>
+      </c>
       <c r="F5" s="3">
         <v>3</v>
       </c>
@@ -567,7 +579,7 @@
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="5">
         <v>1</v>
       </c>
       <c r="F7" s="3">
@@ -582,7 +594,7 @@
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>1</v>
       </c>
       <c r="F8" s="3">
@@ -599,7 +611,7 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F9" s="3">
@@ -614,7 +626,7 @@
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>3</v>
       </c>
       <c r="F10" s="3">
@@ -629,7 +641,7 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <v>1</v>
       </c>
     </row>
@@ -640,7 +652,7 @@
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>2</v>
       </c>
     </row>
@@ -651,7 +663,7 @@
       <c r="B13">
         <v>4</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>4</v>
       </c>
     </row>
@@ -662,7 +674,7 @@
       <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="6" t="s">
         <v>35</v>
       </c>
     </row>
@@ -673,7 +685,7 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -684,7 +696,7 @@
       <c r="B16">
         <v>5</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>5</v>
       </c>
     </row>
@@ -695,7 +707,7 @@
       <c r="B17">
         <v>3</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>3</v>
       </c>
     </row>
@@ -706,7 +718,7 @@
       <c r="B18">
         <v>2</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>2</v>
       </c>
     </row>
@@ -717,8 +729,14 @@
       <c r="B19">
         <v>2</v>
       </c>
-      <c r="C19">
-        <v>2</v>
+      <c r="C19" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="D20">
+        <f>SUM(C7:C19)</f>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="1" customFormat="1">
@@ -736,6 +754,7 @@
       <c r="B22">
         <v>5</v>
       </c>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
@@ -744,6 +763,7 @@
       <c r="B23">
         <v>3</v>
       </c>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
@@ -752,6 +772,7 @@
       <c r="B24">
         <v>3</v>
       </c>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
@@ -760,6 +781,7 @@
       <c r="B25">
         <v>5</v>
       </c>
+      <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
@@ -768,7 +790,7 @@
       <c r="B26">
         <v>5</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="4">
         <v>5</v>
       </c>
     </row>
@@ -779,6 +801,7 @@
       <c r="B27">
         <v>4</v>
       </c>
+      <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
@@ -787,6 +810,7 @@
       <c r="B28">
         <v>10</v>
       </c>
+      <c r="C28" s="4"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
@@ -795,6 +819,15 @@
       <c r="B29">
         <v>5</v>
       </c>
+      <c r="C29" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="D30">
+        <f>SUM(C22:C29)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1">
       <c r="A31" s="1" t="s">
@@ -811,6 +844,7 @@
       <c r="B32">
         <v>2</v>
       </c>
+      <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
@@ -819,6 +853,7 @@
       <c r="B33">
         <v>5</v>
       </c>
+      <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
@@ -827,6 +862,7 @@
       <c r="B34">
         <v>1</v>
       </c>
+      <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
@@ -835,9 +871,14 @@
       <c r="B35">
         <v>2</v>
       </c>
+      <c r="C35" s="4"/>
     </row>
     <row r="36" spans="1:4">
       <c r="C36" s="1"/>
+      <c r="D36">
+        <f>SUM(C32:C35)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1">
       <c r="A37" s="1" t="s">
@@ -845,7 +886,7 @@
       </c>
       <c r="C37">
         <f>SUM(C2:C35)</f>
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D37" s="1">
         <v>100</v>

</xml_diff>

<commit_message>
undo implementiert, hardwareansteuerung iplementiert (fehler beim schreiben)
</commit_message>
<xml_diff>
--- a/Teilaufgaben.xlsx
+++ b/Teilaufgaben.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Hilfefunktion (PDF per Button öffnen)</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>---------</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -480,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -754,7 +760,9 @@
       <c r="B22">
         <v>5</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
@@ -763,7 +771,9 @@
       <c r="B23">
         <v>3</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
@@ -772,7 +782,9 @@
       <c r="B24">
         <v>3</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
@@ -803,7 +815,9 @@
       <c r="B27">
         <v>4</v>
       </c>
-      <c r="C27" s="4"/>
+      <c r="C27" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
@@ -812,7 +826,9 @@
       <c r="B28">
         <v>10</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
@@ -828,7 +844,7 @@
     <row r="30" spans="1:4">
       <c r="D30">
         <f>SUM(C22:C29)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1">
@@ -888,7 +904,7 @@
       </c>
       <c r="C37">
         <f>SUM(C2:C35)</f>
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D37" s="1">
         <v>100</v>

</xml_diff>